<commit_message>
more comparisons in lasso coeff
</commit_message>
<xml_diff>
--- a/cold-start/lasso.xlsx
+++ b/cold-start/lasso.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6480" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="11060" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="ratingsBinary" sheetId="1" r:id="rId1"/>
+    <sheet name="lassos" sheetId="1" r:id="rId1"/>
+    <sheet name="stats" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
   <si>
     <t>wall</t>
   </si>
@@ -76,6 +77,27 @@
   </si>
   <si>
     <t xml:space="preserve"> sears</t>
+  </si>
+  <si>
+    <t>base_fill1</t>
+  </si>
+  <si>
+    <t>sparse%</t>
+  </si>
+  <si>
+    <t>row counts</t>
+  </si>
+  <si>
+    <t>nexxus</t>
+  </si>
+  <si>
+    <t>walmart</t>
+  </si>
+  <si>
+    <t>walls</t>
+  </si>
+  <si>
+    <t>cap@10</t>
   </si>
 </sst>
 </file>
@@ -132,18 +154,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -176,7 +203,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>ratingsBinary!$B$1</c:f>
+              <c:f>lassos!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -187,9 +214,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>ratingsBinary!$A$2:$A$17</c:f>
+              <c:f>lassos!$A$2:$A$18</c:f>
               <c:strCache>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v> master card</c:v>
                 </c:pt>
@@ -237,16 +264,19 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v> sears</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>nexxus</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ratingsBinary!$B$2:$B$17</c:f>
+              <c:f>lassos!$B$2:$B$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>0.2767</c:v>
                 </c:pt>
@@ -294,6 +324,9 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0.0466</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -305,20 +338,20 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>ratingsBinary!$C$1</c:f>
+              <c:f>lassos!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>binary</c:v>
+                  <c:v>base_fill1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>ratingsBinary!$A$2:$A$17</c:f>
+              <c:f>lassos!$A$2:$A$18</c:f>
               <c:strCache>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v> master card</c:v>
                 </c:pt>
@@ -366,16 +399,19 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v> sears</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>nexxus</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ratingsBinary!$C$2:$C$17</c:f>
+              <c:f>lassos!$C$2:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>0.2552</c:v>
                 </c:pt>
@@ -423,11 +459,284 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0.0718</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>lassos!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cap@10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>lassos!$A$2:$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v> master card</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> target</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v> kohls</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v> citiBank USA</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v> McDonalds</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v> VISA signature</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v> Samsung USA</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v> macys</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v> kellogg pop tarts</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v> FRS healthy performance</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v> old navy</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v> CVS</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v> pepsi</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v> charles schwab</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v> Amazon.com</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v> sears</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>nexxus</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>lassos!$D$2:$D$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.0298</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0162</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0646</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0278</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.0113</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0343</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.0455</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.008</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0257</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0476</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.0591</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.0488</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.1449</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.1748</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.129</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0432</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-0.1352</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>lassos!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>binary</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>lassos!$A$2:$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v> master card</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> target</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v> kohls</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v> citiBank USA</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v> McDonalds</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v> VISA signature</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v> Samsung USA</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v> macys</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v> kellogg pop tarts</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v> FRS healthy performance</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v> old navy</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v> CVS</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v> pepsi</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v> charles schwab</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v> Amazon.com</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v> sears</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>nexxus</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>lassos!$E$2:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>-0.1686</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.2498</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.2258</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.1358</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.2665</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.1381</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.2404</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.2631</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-0.179</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.144</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.2793</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.2664</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-0.1041</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.3396</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.3786</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-0.2014</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>-0.1836</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -439,11 +748,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2137326824"/>
-        <c:axId val="2066360216"/>
+        <c:axId val="-2138291944"/>
+        <c:axId val="-2138289816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2137326824"/>
+        <c:axId val="-2138291944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -452,7 +761,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2066360216"/>
+        <c:txPr>
+          <a:bodyPr rot="-5400000" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2138289816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -460,7 +779,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2066360216"/>
+        <c:axId val="-2138289816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.7"/>
@@ -473,7 +792,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2137326824"/>
+        <c:crossAx val="-2138291944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -486,11 +805,21 @@
           <c:yMode val="edge"/>
           <c:x val="0.680148758328286"/>
           <c:y val="0.0898904484765491"/>
-          <c:w val="0.119851241671714"/>
-          <c:h val="0.0831590616390342"/>
+          <c:w val="0.189082010902483"/>
+          <c:h val="0.147341256256011"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -508,16 +837,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -861,18 +1190,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -880,10 +1210,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -893,8 +1229,14 @@
       <c r="C2">
         <v>0.25519999999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <v>2.98E-2</v>
+      </c>
+      <c r="E2">
+        <v>-0.1686</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -904,8 +1246,14 @@
       <c r="C3">
         <v>0.25629999999999997</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3">
+        <v>1.6199999999999999E-2</v>
+      </c>
+      <c r="E3">
+        <v>-0.24979999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -915,8 +1263,14 @@
       <c r="C4">
         <v>0.18390000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4">
+        <v>6.4600000000000005E-2</v>
+      </c>
+      <c r="E4">
+        <v>-0.2258</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -926,8 +1280,14 @@
       <c r="C5">
         <v>3.95E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5">
+        <v>2.7799999999999998E-2</v>
+      </c>
+      <c r="E5">
+        <v>-0.1358</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -937,8 +1297,14 @@
       <c r="C6">
         <v>0.43120000000000003</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6">
+        <v>-1.1299999999999999E-2</v>
+      </c>
+      <c r="E6">
+        <v>-0.26650000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -948,8 +1314,14 @@
       <c r="C7">
         <v>0.31709999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7">
+        <v>3.4299999999999997E-2</v>
+      </c>
+      <c r="E7">
+        <v>-0.1381</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -959,8 +1331,14 @@
       <c r="C8">
         <v>4.53E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8">
+        <v>-4.5499999999999999E-2</v>
+      </c>
+      <c r="E8">
+        <v>-0.2404</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -970,8 +1348,14 @@
       <c r="C9">
         <v>4.87E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E9">
+        <v>-0.2631</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -981,8 +1365,14 @@
       <c r="C10">
         <v>0.29659999999999997</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10">
+        <v>2.5700000000000001E-2</v>
+      </c>
+      <c r="E10">
+        <v>-0.17899999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -992,8 +1382,14 @@
       <c r="C11">
         <v>0.11360000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11">
+        <v>4.7600000000000003E-2</v>
+      </c>
+      <c r="E11">
+        <v>-0.14399999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1003,8 +1399,14 @@
       <c r="C12">
         <v>2.5000000000000001E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12">
+        <v>-5.91E-2</v>
+      </c>
+      <c r="E12">
+        <v>-0.27929999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1014,8 +1416,14 @@
       <c r="C13">
         <v>-2.98E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13">
+        <v>-4.8800000000000003E-2</v>
+      </c>
+      <c r="E13">
+        <v>-0.26640000000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1025,8 +1433,14 @@
       <c r="C14">
         <v>0.2054</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14">
+        <v>0.1449</v>
+      </c>
+      <c r="E14">
+        <v>-0.1041</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1036,8 +1450,14 @@
       <c r="C15">
         <v>-0.41039999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15">
+        <v>-0.17480000000000001</v>
+      </c>
+      <c r="E15">
+        <v>-0.33960000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1047,8 +1467,14 @@
       <c r="C16">
         <v>-3.0599999999999999E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16">
+        <v>-0.129</v>
+      </c>
+      <c r="E16">
+        <v>-0.37859999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1057,6 +1483,29 @@
       </c>
       <c r="C17">
         <v>7.1800000000000003E-2</v>
+      </c>
+      <c r="D17">
+        <v>4.3200000000000002E-2</v>
+      </c>
+      <c r="E17">
+        <v>-0.2014</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>-0.13519999999999999</v>
+      </c>
+      <c r="E18">
+        <v>-0.18360000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1069,4 +1518,233 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2">
+        <v>38390</v>
+      </c>
+      <c r="C2">
+        <v>27.6748511368388</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2821</v>
+      </c>
+      <c r="C3">
+        <v>2.03362216871639</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>45738</v>
+      </c>
+      <c r="C4">
+        <v>32.971928661024499</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>45778</v>
+      </c>
+      <c r="C5">
+        <v>33.0007641401981</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>1966</v>
+      </c>
+      <c r="C6">
+        <v>1.41726380138122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>27691</v>
+      </c>
+      <c r="C7">
+        <v>19.962081344886698</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>2415</v>
+      </c>
+      <c r="C8">
+        <v>1.7409420551046</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>4097</v>
+      </c>
+      <c r="C9">
+        <v>2.9534739543534401</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>36889</v>
+      </c>
+      <c r="C10">
+        <v>26.592799780850399</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>4026</v>
+      </c>
+      <c r="C11">
+        <v>2.9022909788203402</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>2886</v>
+      </c>
+      <c r="C12">
+        <v>2.0804798223734502</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>23343</v>
+      </c>
+      <c r="C13">
+        <v>16.827664758719099</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>14999</v>
+      </c>
+      <c r="C14">
+        <v>10.8125838031113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>25763</v>
+      </c>
+      <c r="C15">
+        <v>18.5722112487204</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>96</v>
+      </c>
+      <c r="C16">
+        <v>6.9205150016580397E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>20449</v>
+      </c>
+      <c r="C17">
+        <v>14.741417840511</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>23445</v>
+      </c>
+      <c r="C18">
+        <v>16.901195230611702</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>36</v>
+      </c>
+      <c r="C19">
+        <v>2.5951931256217701E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding lift to comparison
</commit_message>
<xml_diff>
--- a/cold-start/lasso.xlsx
+++ b/cold-start/lasso.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11060" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500"/>
+    <workbookView xWindow="6960" yWindow="0" windowWidth="25600" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="lassos" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>wall</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>cap@10</t>
+  </si>
+  <si>
+    <t>lift</t>
+  </si>
+  <si>
+    <t>norm_lift</t>
   </si>
 </sst>
 </file>
@@ -154,8 +160,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -166,11 +174,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -199,276 +209,6 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>lassos!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>ratingsdata</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>lassos!$A$2:$A$18</c:f>
-              <c:strCache>
-                <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v> master card</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v> target</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v> kohls</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v> citiBank USA</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v> McDonalds</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v> VISA signature</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v> Samsung USA</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v> macys</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v> kellogg pop tarts</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v> FRS healthy performance</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v> old navy</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v> CVS</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v> pepsi</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v> charles schwab</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v> Amazon.com</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v> sears</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>nexxus</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>lassos!$B$2:$B$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>0.2767</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.3028</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.1872</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0147</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.6472</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.4501</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0369</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0467</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.3752</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.1097</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-0.0003</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-0.0471</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.1921</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-0.939</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.0044</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.0466</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>lassos!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>base_fill1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:strRef>
-              <c:f>lassos!$A$2:$A$18</c:f>
-              <c:strCache>
-                <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v> master card</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v> target</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v> kohls</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v> citiBank USA</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v> McDonalds</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v> VISA signature</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v> Samsung USA</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v> macys</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v> kellogg pop tarts</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v> FRS healthy performance</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v> old navy</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v> CVS</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v> pepsi</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v> charles schwab</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v> Amazon.com</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v> sears</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>nexxus</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>lassos!$C$2:$C$18</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="17"/>
-                <c:pt idx="0">
-                  <c:v>0.2552</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.2563</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.1839</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0395</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.4312</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.3171</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0453</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0487</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.2966</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.1136</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.0025</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-0.0298</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.2054</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-0.4104</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-0.0306</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.0718</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="1"/>
-        </c:ser>
-        <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
@@ -732,6 +472,411 @@
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>-0.1836</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>lassos!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>base_fill1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>lassos!$A$2:$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v> master card</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> target</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v> kohls</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v> citiBank USA</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v> McDonalds</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v> VISA signature</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v> Samsung USA</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v> macys</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v> kellogg pop tarts</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v> FRS healthy performance</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v> old navy</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v> CVS</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v> pepsi</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v> charles schwab</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v> Amazon.com</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v> sears</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>nexxus</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>lassos!$C$2:$C$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.2552</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2563</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1839</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0395</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4312</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3171</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0453</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0487</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2966</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1136</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.0025</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.0298</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.2054</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.4104</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-0.0306</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0718</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>lassos!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ratingsdata</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>lassos!$A$2:$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v> master card</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> target</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v> kohls</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v> citiBank USA</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v> McDonalds</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v> VISA signature</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v> Samsung USA</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v> macys</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v> kellogg pop tarts</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v> FRS healthy performance</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v> old navy</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v> CVS</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v> pepsi</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v> charles schwab</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v> Amazon.com</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v> sears</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>nexxus</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>lassos!$B$2:$B$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.2767</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3028</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1872</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0147</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6472</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.4501</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0369</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0467</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3752</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1097</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.0003</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-0.0471</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.1921</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-0.939</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.0044</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.0466</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>lassos!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>norm_lift</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>lassos!$A$2:$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v> master card</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> target</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v> kohls</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v> citiBank USA</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v> McDonalds</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v> VISA signature</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v> Samsung USA</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v> macys</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v> kellogg pop tarts</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v> FRS healthy performance</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v> old navy</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v> CVS</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v> pepsi</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v> charles schwab</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v> Amazon.com</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v> sears</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>nexxus</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>lassos!$F$2:$F$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.592</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.576</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.576</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.552</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.496</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.488</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.432</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.408</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.392</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.384</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.376</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.336</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.304</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.288</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.28</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.272</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.272</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -803,10 +948,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.680148758328286"/>
-          <c:y val="0.0898904484765491"/>
-          <c:w val="0.189082010902483"/>
-          <c:h val="0.147341256256011"/>
+          <c:x val="0.0583636103732116"/>
+          <c:y val="0.643745992820316"/>
+          <c:w val="0.234467818981024"/>
+          <c:h val="0.323316984532656"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -837,16 +982,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>215900</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1190,10 +1335,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1202,7 +1347,7 @@
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1218,8 +1363,11 @@
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1235,8 +1383,12 @@
       <c r="E2">
         <v>-0.1686</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <f>E21/125</f>
+        <v>0.59199999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1252,8 +1404,12 @@
       <c r="E3">
         <v>-0.24979999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3">
+        <f t="shared" ref="F3:F18" si="0">E22/125</f>
+        <v>0.57599999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1269,8 +1425,12 @@
       <c r="E4">
         <v>-0.2258</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0.57599999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1286,8 +1446,12 @@
       <c r="E5">
         <v>-0.1358</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0.55200000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1303,8 +1467,12 @@
       <c r="E6">
         <v>-0.26650000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0.496</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1320,8 +1488,12 @@
       <c r="E7">
         <v>-0.1381</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>0.48799999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1337,8 +1509,12 @@
       <c r="E8">
         <v>-0.2404</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0.432</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1354,8 +1530,12 @@
       <c r="E9">
         <v>-0.2631</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0.40799999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1371,8 +1551,12 @@
       <c r="E10">
         <v>-0.17899999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0.39200000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1388,8 +1572,12 @@
       <c r="E11">
         <v>-0.14399999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0.38400000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1405,8 +1593,12 @@
       <c r="E12">
         <v>-0.27929999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0.376</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1422,8 +1614,12 @@
       <c r="E13">
         <v>-0.26640000000000003</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0.33600000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1439,8 +1635,12 @@
       <c r="E14">
         <v>-0.1041</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>0.30399999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1456,8 +1656,12 @@
       <c r="E15">
         <v>-0.33960000000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>0.28799999999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1473,8 +1677,12 @@
       <c r="E16">
         <v>-0.37859999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1490,8 +1698,12 @@
       <c r="E17">
         <v>-0.2014</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>0.27200000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1506,6 +1718,100 @@
       </c>
       <c r="E18">
         <v>-0.18360000000000001</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>0.27200000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="E21">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="E22">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="E23">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="E24">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="E25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="E26">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="E27">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="E28">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="E29">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="E30">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="E31">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="E32">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="5:5">
+      <c r="E33">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5">
+      <c r="E34">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5">
+      <c r="E35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5">
+      <c r="E36">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="5:5">
+      <c r="E37">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1525,7 +1831,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>